<commit_message>
Added FileOutputStream to write data to user list after user creation Removed unnecisary Eclipse files Added stop command (Main is now in a loop) Removed debug code
</commit_message>
<xml_diff>
--- a/demosheet.xlsx
+++ b/demosheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\tagIn\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eclipse\TagIn-Java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47162CC4-FDCA-46CD-9ECA-91842BE33411}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6485F197-5E25-4142-8C1B-B5A95CE2F486}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4540" yWindow="3727" windowWidth="14400" windowHeight="10073" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -344,7 +344,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>

</xml_diff>

<commit_message>
Added the "find" command which can find a users UUID, name, and row in the list using either the users UUID or name
</commit_message>
<xml_diff>
--- a/demosheet.xlsx
+++ b/demosheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eclipse\TagIn-Java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6485F197-5E25-4142-8C1B-B5A95CE2F486}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48145AB3-4E23-4BE6-89F2-3F097867F066}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4540" yWindow="3727" windowWidth="14400" windowHeight="10073" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -344,7 +344,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>

</xml_diff>

<commit_message>
Populated demosheet (current user list file) with makeshift team members thanks matt.
</commit_message>
<xml_diff>
--- a/demosheet.xlsx
+++ b/demosheet.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eclipse\TagIn-Java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48145AB3-4E23-4BE6-89F2-3F097867F066}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{48145AB3-4E23-4BE6-89F2-3F097867F066}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView xWindow="4540" yWindow="3727" windowWidth="14400" windowHeight="10073" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="10073" windowWidth="14400" xWindow="4540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="3727"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,11 +25,142 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
+  <si>
+    <t>7b9df9ee-a516-4cdd-bff0-e342bbfbed61</t>
+  </si>
+  <si>
+    <t>Aidan</t>
+  </si>
+  <si>
+    <t>12:00 AM</t>
+  </si>
+  <si>
+    <t>e5225aa7-ebc6-40d3-9f28-8c05cbf10689</t>
+  </si>
+  <si>
+    <t>Amrit</t>
+  </si>
+  <si>
+    <t>e4b817ae-5800-4606-a201-549bc52b92f1</t>
+  </si>
+  <si>
+    <t>Anna</t>
+  </si>
+  <si>
+    <t>5b0d086b-a7a5-4ed0-97d7-81e194c293bb</t>
+  </si>
+  <si>
+    <t>Ben</t>
+  </si>
+  <si>
+    <t>45c1f085-80fc-4432-895c-e63e6a7b10cc</t>
+  </si>
+  <si>
+    <t>Camila</t>
+  </si>
+  <si>
+    <t>3a33eceb-6250-4088-990d-ca071a926d60</t>
+  </si>
+  <si>
+    <t>Charlotte</t>
+  </si>
+  <si>
+    <t>bd7cf070-1afb-49b8-84dc-72bd69e4c70c</t>
+  </si>
+  <si>
+    <t>Claudia</t>
+  </si>
+  <si>
+    <t>ba102f8a-a9c5-4cff-a481-6d5f90a3d920</t>
+  </si>
+  <si>
+    <t>Connor</t>
+  </si>
+  <si>
+    <t>b663afcb-c6df-4617-b020-ec27e427356a</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>79eb5a64-41c9-4aca-879c-363bd4dece00</t>
+  </si>
+  <si>
+    <t>Edward</t>
+  </si>
+  <si>
+    <t>a92a085b-e1ee-465b-8f5c-2bae94542872</t>
+  </si>
+  <si>
+    <t>Jackson</t>
+  </si>
+  <si>
+    <t>c00f9d5b-2f12-4c47-adf8-e0ae5f836e07</t>
+  </si>
+  <si>
+    <t>Jaeson</t>
+  </si>
+  <si>
+    <t>baabaf26-f689-4afe-8573-cec87477ccf2</t>
+  </si>
+  <si>
+    <t>Liam</t>
+  </si>
+  <si>
+    <t>c7ef5a3f-f2d2-4c4e-b198-1b63bb8ba4d1</t>
+  </si>
+  <si>
+    <t>Michael A</t>
+  </si>
+  <si>
+    <t>9e743881-ae7e-4e7b-a2a4-271e86bb6805</t>
+  </si>
+  <si>
+    <t>Michael T</t>
+  </si>
+  <si>
+    <t>e48ffff2-1487-4224-8d4f-40804a1e18de</t>
+  </si>
+  <si>
+    <t>Nicholas</t>
+  </si>
+  <si>
+    <t>fd578fd8-c955-4e7c-91a1-5cb4e8c5be8e</t>
+  </si>
+  <si>
+    <t>Remy</t>
+  </si>
+  <si>
+    <t>e1a12057-e28a-48f0-b179-b064ec105871</t>
+  </si>
+  <si>
+    <t>Valentina</t>
+  </si>
+  <si>
+    <t>d077018e-e68b-4027-8d98-b2637c408c8f</t>
+  </si>
+  <si>
+    <t>Vikram</t>
+  </si>
+  <si>
+    <t>21e1b9c9-a2b8-4cdc-9c94-0b38a4d4c78e</t>
+  </si>
+  <si>
+    <t>William</t>
+  </si>
+  <si>
+    <t>c83d884c-983f-40c5-b794-423f00aec95a</t>
+  </si>
+  <si>
+    <t>Zaid</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -57,16 +188,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -83,10 +214,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -121,7 +252,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -156,7 +287,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -250,21 +381,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -281,7 +412,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -333,22 +464,317 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" t="b">
+        <v>0</v>
+      </c>
+      <c r="D20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" t="b">
+        <v>0</v>
+      </c>
+      <c r="D21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Removed sign-in/out time as it is unneeded for the current attendance spreadsheet Fixed an issue with the"find" command which would cause a NPE if a user's name or uuid was not found
</commit_message>
<xml_diff>
--- a/demosheet.xlsx
+++ b/demosheet.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eclipse\TagIn-Java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{48145AB3-4E23-4BE6-89F2-3F097867F066}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE89D41-35D9-4370-9D78-DBE30F0A5FFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="10073" windowWidth="14400" xWindow="4540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="3727"/>
+    <workbookView xWindow="10050" yWindow="2730" windowWidth="13680" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>7b9df9ee-a516-4cdd-bff0-e342bbfbed61</t>
   </si>
   <si>
     <t>Aidan</t>
-  </si>
-  <si>
-    <t>12:00 AM</t>
   </si>
   <si>
     <t>e5225aa7-ebc6-40d3-9f28-8c05cbf10689</t>
@@ -160,7 +157,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -188,16 +184,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -214,10 +210,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -252,7 +248,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -287,7 +283,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -381,21 +377,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -412,7 +408,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -464,23 +460,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B3"/>
+      <selection activeCell="D1" sqref="D1:D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -490,291 +486,228 @@
       <c r="C1" t="b">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="C8" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="C9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>20</v>
       </c>
-      <c r="C10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
         <v>21</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>22</v>
       </c>
-      <c r="C11" t="b">
-        <v>0</v>
-      </c>
-      <c r="D11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
         <v>23</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>24</v>
       </c>
-      <c r="C12" t="b">
-        <v>0</v>
-      </c>
-      <c r="D12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
         <v>25</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>26</v>
       </c>
-      <c r="C13" t="b">
-        <v>0</v>
-      </c>
-      <c r="D13" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
         <v>27</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>28</v>
       </c>
-      <c r="C14" t="b">
-        <v>0</v>
-      </c>
-      <c r="D14" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
         <v>29</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>30</v>
       </c>
-      <c r="C15" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
         <v>31</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>32</v>
       </c>
-      <c r="C16" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
         <v>33</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>34</v>
       </c>
-      <c r="C17" t="b">
-        <v>0</v>
-      </c>
-      <c r="D17" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
         <v>35</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>36</v>
       </c>
-      <c r="C18" t="b">
-        <v>0</v>
-      </c>
-      <c r="D18" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
         <v>37</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>38</v>
       </c>
-      <c r="C19" t="b">
-        <v>0</v>
-      </c>
-      <c r="D19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
         <v>39</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>40</v>
       </c>
-      <c r="C20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D20" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
+      <c r="B21" t="s">
         <v>41</v>
       </c>
-      <c r="B21" t="s">
-        <v>42</v>
-      </c>
       <c r="C21" t="b">
         <v>0</v>
       </c>
-      <c r="D21" t="s">
-        <v>2</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>